<commit_message>
excel to ppt initial
</commit_message>
<xml_diff>
--- a/tamil_biology/002_NEET_Questions.xlsx
+++ b/tamil_biology/002_NEET_Questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\2020\git\tvmani.github.io\tamil_biology\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E653B20-8DD3-4398-93B1-64357CED46A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33507521-A89D-4A50-A884-12D73A6D4D5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{10B15D36-62A2-42E1-96B8-002C7E680664}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>question_no</t>
   </si>
@@ -57,18 +57,6 @@
     <t>எண்டோபிளாச வலை</t>
   </si>
   <si>
-    <t xml:space="preserve">மைட்டோகாண்டிரியாவின் உட்சவ்வு </t>
-  </si>
-  <si>
-    <t>மைட்டோகாண்டிரியாவின் வெளிச்சவ்வு</t>
-  </si>
-  <si>
-    <t xml:space="preserve">கிரானம் </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ஸ்ட்ரோமா </t>
-  </si>
-  <si>
     <t>correct_answer</t>
   </si>
   <si>
@@ -82,9 +70,6 @@
   </si>
   <si>
     <t>குவான்டோசோம் இவற்றில் காணப்படுகிறது?</t>
-  </si>
-  <si>
-    <t>சைட்டோகுரோம் ஆக்ஸிடேஸ் என்ற நொதி மைட்டோகாண்டிரியாவில் காணப்படும் இடம்?</t>
   </si>
 </sst>
 </file>
@@ -116,7 +101,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -200,46 +185,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -262,20 +212,211 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="14">
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -305,206 +446,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -519,18 +460,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8E3837A6-55E6-4161-B295-E35C1DE28112}" name="biology_neet_2020" displayName="biology_neet_2020" ref="A1:I3" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" headerRowBorderDxfId="12" tableBorderDxfId="13" totalsRowBorderDxfId="11">
-  <autoFilter ref="A1:I3" xr:uid="{21C90CC8-F43A-4449-ACD8-A4A8B496274B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8E3837A6-55E6-4161-B295-E35C1DE28112}" name="biology_neet_2020" displayName="biology_neet_2020" ref="A1:I2" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10" totalsRowBorderDxfId="9">
+  <autoFilter ref="A1:I2" xr:uid="{21C90CC8-F43A-4449-ACD8-A4A8B496274B}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{6FA8DE45-DBFC-4EBF-8D34-F711DDA988BF}" name="question_no" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{B8A938FA-0587-441C-8D44-21199B236420}" name="question" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{E1DBB7D1-74B4-45DB-928C-6AA0316F57C4}" name="exams_already_asked" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{E1246A8C-A829-43D9-A2FD-269863315184}" name="year" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{C77BB146-B5EE-4A08-A7E5-15C0881CD1F1}" name="option_1" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{4CBD5902-0360-4375-B9D8-2C0CDB5595C1}" name="option_2" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{E9AA603F-7891-4008-8A74-D495626F4D19}" name="option_3" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{CE3CE54D-5CD9-45D6-94DA-40F1AF3D1C8F}" name="option_4" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{5BA1AA38-E0EA-4ADC-A77D-56B66F6A3E24}" name="correct_answer" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{6FA8DE45-DBFC-4EBF-8D34-F711DDA988BF}" name="question_no" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{B8A938FA-0587-441C-8D44-21199B236420}" name="question" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{E1DBB7D1-74B4-45DB-928C-6AA0316F57C4}" name="exams_already_asked" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{E1246A8C-A829-43D9-A2FD-269863315184}" name="year" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{C77BB146-B5EE-4A08-A7E5-15C0881CD1F1}" name="option_1" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{4CBD5902-0360-4375-B9D8-2C0CDB5595C1}" name="option_2" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{E9AA603F-7891-4008-8A74-D495626F4D19}" name="option_3" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{CE3CE54D-5CD9-45D6-94DA-40F1AF3D1C8F}" name="option_4" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{5BA1AA38-E0EA-4ADC-A77D-56B66F6A3E24}" name="correct_answer" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -833,7 +774,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAEBE3C3-D3AB-45CC-A447-DC1A39997F74}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
@@ -859,10 +800,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>2</v>
@@ -877,7 +818,7 @@
         <v>5</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -885,10 +826,10 @@
         <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D2" s="2">
         <v>2012</v>
@@ -906,35 +847,6 @@
         <v>9</v>
       </c>
       <c r="I2" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="8">
-        <v>8</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="9">
-        <v>2012</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="10">
         <v>2</v>
       </c>
     </row>

</xml_diff>